<commit_message>
2 best linear reg on data based on r value
</commit_message>
<xml_diff>
--- a/testvalues.xlsx
+++ b/testvalues.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23515"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="2920" yWindow="0" windowWidth="24300" windowHeight="15320" tabRatio="500"/>
+    <workbookView xWindow="5340" yWindow="0" windowWidth="25140" windowHeight="15620" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,12 +18,39 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+  <si>
+    <t>index 20</t>
+  </si>
+  <si>
+    <t>index 29</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -46,13 +73,21 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="5">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -382,10 +417,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B30"/>
+  <dimension ref="A1:C30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -403,7 +438,7 @@
         <v>2</v>
       </c>
       <c r="B2">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -411,7 +446,7 @@
         <v>3</v>
       </c>
       <c r="B3">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -419,7 +454,7 @@
         <v>4</v>
       </c>
       <c r="B4">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -427,7 +462,7 @@
         <v>5</v>
       </c>
       <c r="B5">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -435,7 +470,7 @@
         <v>6</v>
       </c>
       <c r="B6">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -443,7 +478,7 @@
         <v>7</v>
       </c>
       <c r="B7">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -451,7 +486,7 @@
         <v>8</v>
       </c>
       <c r="B8">
-        <v>14</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -459,7 +494,7 @@
         <v>9</v>
       </c>
       <c r="B9">
-        <v>16</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -467,7 +502,7 @@
         <v>10</v>
       </c>
       <c r="B10">
-        <v>17</v>
+        <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -475,7 +510,7 @@
         <v>11</v>
       </c>
       <c r="B11">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -483,7 +518,7 @@
         <v>12</v>
       </c>
       <c r="B12">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -491,7 +526,7 @@
         <v>13</v>
       </c>
       <c r="B13">
-        <v>20</v>
+        <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -499,7 +534,7 @@
         <v>14</v>
       </c>
       <c r="B14">
-        <v>24</v>
+        <v>13</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -507,7 +542,7 @@
         <v>15</v>
       </c>
       <c r="B15">
-        <v>26</v>
+        <v>16</v>
       </c>
     </row>
     <row r="16" spans="1:2">
@@ -515,123 +550,130 @@
         <v>16</v>
       </c>
       <c r="B16">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
       <c r="A17">
         <v>17</v>
       </c>
       <c r="B17">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
       <c r="A18">
         <v>18</v>
       </c>
       <c r="B18">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
       <c r="A19">
         <v>19</v>
       </c>
       <c r="B19">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
       <c r="A20">
         <v>20</v>
       </c>
       <c r="B20">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
       <c r="A21">
         <v>21</v>
       </c>
       <c r="B21">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2">
+        <v>32</v>
+      </c>
+      <c r="C21" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
       <c r="A22">
         <v>22</v>
       </c>
       <c r="B22">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
       <c r="A23">
         <v>23</v>
       </c>
       <c r="B23">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
       <c r="A24">
         <v>24</v>
       </c>
       <c r="B24">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
       <c r="A25">
         <v>25</v>
       </c>
       <c r="B25">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
       <c r="A26">
         <v>26</v>
       </c>
       <c r="B26">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
       <c r="A27">
         <v>27</v>
       </c>
       <c r="B27">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
       <c r="A28">
         <v>28</v>
       </c>
       <c r="B28">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
       <c r="A29">
         <v>29</v>
       </c>
       <c r="B29">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
       <c r="A30">
         <v>30</v>
       </c>
       <c r="B30">
-        <v>98</v>
+        <v>50</v>
+      </c>
+      <c r="C30" t="s">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>